<commit_message>
Update: Improve popup text size and detailed descriptions
</commit_message>
<xml_diff>
--- a/business_trips_2025_analyzed.xlsx
+++ b/business_trips_2025_analyzed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
   <si>
     <t>보고서ID</t>
   </si>
@@ -73,6 +73,12 @@
     <t>충북</t>
   </si>
   <si>
+    <t>대구시</t>
+  </si>
+  <si>
+    <t>전남</t>
+  </si>
+  <si>
     <t>김천시</t>
   </si>
   <si>
@@ -100,6 +106,12 @@
     <t>고창군</t>
   </si>
   <si>
+    <t>밀양</t>
+  </si>
+  <si>
+    <t>해남군</t>
+  </si>
+  <si>
     <t>사과 출하 독려</t>
   </si>
   <si>
@@ -121,6 +133,15 @@
     <t>상추, 깻잎 출하 독려</t>
   </si>
   <si>
+    <t>참외 작목현황</t>
+  </si>
+  <si>
+    <t>하우스감사 시세 동향 및 출하 상담</t>
+  </si>
+  <si>
+    <t>봄동배추, 대파 줄하독려</t>
+  </si>
+  <si>
     <t>윤정기, 이광진</t>
   </si>
   <si>
@@ -139,6 +160,15 @@
     <t>김득중, 김언중</t>
   </si>
   <si>
+    <t>김상걸, 차수호</t>
+  </si>
+  <si>
+    <t>김용보, 이용수</t>
+  </si>
+  <si>
+    <t>김언중 김기영</t>
+  </si>
+  <si>
     <t>사과 작목반</t>
   </si>
   <si>
@@ -163,6 +193,15 @@
     <t>상추, 깻잎</t>
   </si>
   <si>
+    <t xml:space="preserve">참외 </t>
+  </si>
+  <si>
+    <t>감자</t>
+  </si>
+  <si>
+    <t>배추,대파</t>
+  </si>
+  <si>
     <t>윤정기</t>
   </si>
   <si>
@@ -176,6 +215,12 @@
   </si>
   <si>
     <t>김득중</t>
+  </si>
+  <si>
+    <t>김상걸</t>
+  </si>
+  <si>
+    <t>김용보</t>
   </si>
 </sst>
 </file>
@@ -537,7 +582,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -595,22 +640,22 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="J2" s="2">
         <v>45665</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -630,22 +675,22 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J3" s="2">
         <v>45666</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -665,22 +710,22 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="J4" s="2">
         <v>45667</v>
       </c>
       <c r="K4" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -700,22 +745,22 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J5" s="2">
         <v>45671</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -735,22 +780,22 @@
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J6" s="2">
         <v>45672</v>
       </c>
       <c r="K6" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -770,22 +815,22 @@
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="J7" s="2">
         <v>45673</v>
       </c>
       <c r="K7" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -805,22 +850,22 @@
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="J8" s="2">
         <v>45673</v>
       </c>
       <c r="K8" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -840,22 +885,22 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I9" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="J9" s="2">
         <v>45675</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -875,22 +920,22 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="J10" s="2">
         <v>45675</v>
       </c>
       <c r="K10" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -910,22 +955,22 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="I11" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="J11" s="2">
         <v>45675</v>
       </c>
       <c r="K11" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -945,22 +990,127 @@
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I12" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="J12" s="2">
         <v>45678</v>
       </c>
       <c r="K12" t="s">
-        <v>53</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45693</v>
+      </c>
+      <c r="C13" s="2">
+        <v>45693</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="2">
+        <v>45694</v>
+      </c>
+      <c r="K13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45693</v>
+      </c>
+      <c r="C14" s="2">
+        <v>45693</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="2">
+        <v>45694</v>
+      </c>
+      <c r="K14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45693</v>
+      </c>
+      <c r="C15" s="2">
+        <v>45693</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="2">
+        <v>45694</v>
+      </c>
+      <c r="K15" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>